<commit_message>
Processors: Performance: Overclocking: Add VBS off
</commit_message>
<xml_diff>
--- a/Processors/Performance/Overclocking.xlsx
+++ b/Processors/Performance/Overclocking.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="43" uniqueCount="25">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="46" uniqueCount="26">
   <si>
     <t>新乐士 DDR5 32G 6400MHz CL32 *2 + EXPO 2 + MSI HEM Tightest</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -117,6 +117,10 @@
   </si>
   <si>
     <t>VDDCR_VDD</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>PBO Enhanced 3 + VBS off</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -402,10 +406,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:Q22"/>
+  <dimension ref="A1:Q25"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
-      <selection activeCell="L22" sqref="L22"/>
+      <selection activeCell="K20" sqref="K20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
@@ -489,11 +493,11 @@
         <v>51639</v>
       </c>
       <c r="I2">
-        <f t="shared" ref="I2:I22" si="0">G2/E2</f>
+        <f t="shared" ref="I2:I25" si="0">G2/E2</f>
         <v>12.147494707127734</v>
       </c>
       <c r="J2">
-        <f t="shared" ref="J2:J22" si="1">G2/12</f>
+        <f t="shared" ref="J2:J25" si="1">G2/12</f>
         <v>4303.25</v>
       </c>
     </row>
@@ -669,14 +673,14 @@
         <v>4401</v>
       </c>
       <c r="F8" s="2">
-        <f t="shared" ref="F8:F22" si="6">E8/$E$3</f>
+        <f t="shared" ref="F8:F25" si="6">E8/$E$3</f>
         <v>1.0277907519850538</v>
       </c>
       <c r="G8">
         <v>54967</v>
       </c>
       <c r="H8" s="2">
-        <f t="shared" ref="H8:H22" si="7">G8/$G$3</f>
+        <f t="shared" ref="H8:H25" si="7">G8/$G$3</f>
         <v>1.0312951462503988</v>
       </c>
       <c r="I8">
@@ -707,11 +711,11 @@
         <v>1.041989530760427</v>
       </c>
       <c r="I9">
-        <f t="shared" ref="I9:I19" si="8">G9/E9</f>
+        <f t="shared" ref="I9:I22" si="8">G9/E9</f>
         <v>12.610581289736603</v>
       </c>
       <c r="J9">
-        <f t="shared" ref="J9:J19" si="9">G9/12</f>
+        <f t="shared" ref="J9:J22" si="9">G9/12</f>
         <v>4628.083333333333</v>
       </c>
     </row>
@@ -945,83 +949,83 @@
     </row>
     <row r="16" spans="1:17" x14ac:dyDescent="0.3">
       <c r="D16" t="s">
-        <v>19</v>
+        <v>25</v>
       </c>
       <c r="E16">
         <v>4443</v>
       </c>
       <c r="F16" s="2">
-        <f>E16/$E$3</f>
+        <f t="shared" si="6"/>
         <v>1.037599252685661</v>
       </c>
       <c r="G16">
-        <v>55508</v>
+        <v>55650</v>
       </c>
       <c r="H16" s="2">
         <f t="shared" si="7"/>
-        <v>1.0414454304958818</v>
+        <v>1.0441096455843448</v>
       </c>
       <c r="I16">
         <f t="shared" si="8"/>
-        <v>12.493360342111187</v>
+        <v>12.525320729237002</v>
       </c>
       <c r="J16">
         <f t="shared" si="9"/>
-        <v>4625.666666666667</v>
+        <v>4637.5</v>
       </c>
     </row>
     <row r="17" spans="1:17" x14ac:dyDescent="0.3">
       <c r="D17" t="s">
-        <v>19</v>
+        <v>25</v>
       </c>
       <c r="E17">
-        <v>4441</v>
+        <v>4438</v>
       </c>
       <c r="F17" s="2">
-        <f>E17/$E$3</f>
-        <v>1.0371321812237273</v>
+        <f t="shared" si="6"/>
+        <v>1.0364315740308268</v>
       </c>
       <c r="G17">
-        <v>55416</v>
+        <v>55739</v>
       </c>
       <c r="H17" s="2">
         <f t="shared" si="7"/>
-        <v>1.0397193193118071</v>
+        <v>1.0457794705341563</v>
       </c>
       <c r="I17">
         <f t="shared" si="8"/>
-        <v>12.478270659761314</v>
+        <v>12.559486255069851</v>
       </c>
       <c r="J17">
         <f t="shared" si="9"/>
-        <v>4618</v>
+        <v>4644.916666666667</v>
       </c>
     </row>
     <row r="18" spans="1:17" x14ac:dyDescent="0.3">
       <c r="D18" t="s">
-        <v>19</v>
+        <v>25</v>
       </c>
       <c r="E18">
-        <v>4446</v>
+        <v>4439</v>
       </c>
       <c r="F18" s="2">
-        <f>E18/$E$3</f>
-        <v>1.0382998598785613</v>
+        <f t="shared" si="6"/>
+        <v>1.0366651097617936</v>
       </c>
       <c r="G18">
-        <v>55399</v>
+        <v>55610</v>
       </c>
       <c r="H18" s="2">
         <f t="shared" si="7"/>
-        <v>1.039400363984315</v>
+        <v>1.0433591624608343</v>
       </c>
       <c r="I18">
         <f t="shared" si="8"/>
-        <v>12.460413855150698</v>
+        <v>12.527596305474207</v>
       </c>
       <c r="J18">
         <f t="shared" si="9"/>
-        <v>4616.583333333333</v>
+        <v>4634.166666666667</v>
       </c>
     </row>
     <row r="19" spans="1:17" x14ac:dyDescent="0.3">
@@ -1029,118 +1033,199 @@
         <v>19</v>
       </c>
       <c r="E19">
-        <v>4364</v>
+        <v>4443</v>
       </c>
       <c r="F19" s="2">
         <f>E19/$E$3</f>
-        <v>1.0191499299392808</v>
+        <v>1.037599252685661</v>
       </c>
       <c r="G19">
-        <v>54002</v>
+        <v>55508</v>
       </c>
       <c r="H19" s="2">
         <f t="shared" si="7"/>
-        <v>1.0131897408957016</v>
+        <v>1.0414454304958818</v>
       </c>
       <c r="I19">
         <f t="shared" si="8"/>
-        <v>12.374427131072411</v>
+        <v>12.493360342111187</v>
       </c>
       <c r="J19">
         <f t="shared" si="9"/>
+        <v>4625.666666666667</v>
+      </c>
+    </row>
+    <row r="20" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="D20" t="s">
+        <v>19</v>
+      </c>
+      <c r="E20">
+        <v>4441</v>
+      </c>
+      <c r="F20" s="2">
+        <f>E20/$E$3</f>
+        <v>1.0371321812237273</v>
+      </c>
+      <c r="G20">
+        <v>55416</v>
+      </c>
+      <c r="H20" s="2">
+        <f t="shared" si="7"/>
+        <v>1.0397193193118071</v>
+      </c>
+      <c r="I20">
+        <f t="shared" si="8"/>
+        <v>12.478270659761314</v>
+      </c>
+      <c r="J20">
+        <f t="shared" si="9"/>
+        <v>4618</v>
+      </c>
+    </row>
+    <row r="21" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="D21" t="s">
+        <v>19</v>
+      </c>
+      <c r="E21">
+        <v>4446</v>
+      </c>
+      <c r="F21" s="2">
+        <f>E21/$E$3</f>
+        <v>1.0382998598785613</v>
+      </c>
+      <c r="G21">
+        <v>55399</v>
+      </c>
+      <c r="H21" s="2">
+        <f t="shared" si="7"/>
+        <v>1.039400363984315</v>
+      </c>
+      <c r="I21">
+        <f t="shared" si="8"/>
+        <v>12.460413855150698</v>
+      </c>
+      <c r="J21">
+        <f t="shared" si="9"/>
+        <v>4616.583333333333</v>
+      </c>
+    </row>
+    <row r="22" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="D22" t="s">
+        <v>19</v>
+      </c>
+      <c r="E22">
+        <v>4364</v>
+      </c>
+      <c r="F22" s="2">
+        <f>E22/$E$3</f>
+        <v>1.0191499299392808</v>
+      </c>
+      <c r="G22">
+        <v>54002</v>
+      </c>
+      <c r="H22" s="2">
+        <f t="shared" si="7"/>
+        <v>1.0131897408957016</v>
+      </c>
+      <c r="I22">
+        <f t="shared" si="8"/>
+        <v>12.374427131072411</v>
+      </c>
+      <c r="J22">
+        <f t="shared" si="9"/>
         <v>4500.166666666667</v>
       </c>
-      <c r="K19">
+      <c r="K22">
         <v>1.48</v>
       </c>
-      <c r="M19">
+      <c r="M22">
         <v>108.6</v>
       </c>
-      <c r="N19">
+      <c r="N22">
         <v>209</v>
       </c>
-      <c r="O19" s="2">
-        <f>N19/$N$5</f>
+      <c r="O22" s="2">
+        <f>N22/$N$5</f>
         <v>1.2222222222222223</v>
       </c>
-      <c r="P19">
+      <c r="P22">
         <v>204</v>
       </c>
-      <c r="Q19" s="2">
-        <f>P19/$P$5</f>
+      <c r="Q22" s="2">
+        <f>P22/$P$5</f>
         <v>1.2157330154946364</v>
       </c>
     </row>
-    <row r="20" spans="1:17" x14ac:dyDescent="0.3">
-      <c r="D20" s="3" t="s">
+    <row r="23" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="D23" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="E20" s="3"/>
-      <c r="F20" s="4"/>
-      <c r="G20" s="3"/>
-      <c r="H20" s="4"/>
-      <c r="I20" s="3"/>
-      <c r="J20" s="3"/>
-    </row>
-    <row r="21" spans="1:17" x14ac:dyDescent="0.3">
-      <c r="D21" s="3" t="s">
+      <c r="E23" s="3"/>
+      <c r="F23" s="4"/>
+      <c r="G23" s="3"/>
+      <c r="H23" s="4"/>
+      <c r="I23" s="3"/>
+      <c r="J23" s="3"/>
+    </row>
+    <row r="24" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="D24" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="E21" s="3">
+      <c r="E24" s="3">
         <v>4460</v>
       </c>
-      <c r="F21" s="4">
+      <c r="F24" s="4">
         <f t="shared" si="6"/>
         <v>1.0415693601120972</v>
       </c>
-      <c r="G21" s="3">
+      <c r="G24" s="3">
         <v>55826</v>
       </c>
-      <c r="H21" s="4">
+      <c r="H24" s="4">
         <f t="shared" si="7"/>
         <v>1.0474117713277922</v>
       </c>
-      <c r="I21" s="3">
+      <c r="I24" s="3">
         <f t="shared" si="0"/>
         <v>12.517040358744394</v>
       </c>
-      <c r="J21" s="3">
+      <c r="J24" s="3">
         <f t="shared" si="1"/>
         <v>4652.166666666667</v>
       </c>
     </row>
-    <row r="22" spans="1:17" x14ac:dyDescent="0.3">
-      <c r="A22" t="s">
+    <row r="25" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="A25" t="s">
         <v>14</v>
       </c>
-      <c r="B22" s="1" t="s">
+      <c r="B25" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="C22" s="1" t="s">
+      <c r="C25" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="D22" t="s">
+      <c r="D25" t="s">
         <v>15</v>
       </c>
-      <c r="E22">
+      <c r="E25">
         <v>4689</v>
       </c>
-      <c r="F22" s="2">
+      <c r="F25" s="2">
         <f t="shared" si="6"/>
         <v>1.0950490425035031</v>
       </c>
-      <c r="G22">
+      <c r="G25">
         <v>54839</v>
       </c>
-      <c r="H22" s="2">
+      <c r="H25" s="2">
         <f t="shared" si="7"/>
         <v>1.0288936002551643</v>
       </c>
-      <c r="I22">
+      <c r="I25">
         <f t="shared" si="0"/>
         <v>11.695244188526338</v>
       </c>
-      <c r="J22">
+      <c r="J25">
         <f t="shared" si="1"/>
         <v>4569.916666666667</v>
       </c>

</xml_diff>